<commit_message>
Apsimx Intermediate Wheatgrass verson used for paper submitted to the European Journal of Agronomy
</commit_message>
<xml_diff>
--- a/Prototypes/IntermediateWheatgrass/Observed.xlsx
+++ b/Prototypes/IntermediateWheatgrass/Observed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\USQ\PetesPapers\Thesis\Chapter5 PG Model\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B8F589-3DC8-4142-9A99-396421A8044C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6541F6D2-A841-4E36-8CCC-1E3552145CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="960" windowWidth="21040" windowHeight="14390" tabRatio="765" xr2:uid="{CD11C47C-4470-47D7-8492-EF1E35E170CD}"/>
+    <workbookView xWindow="530" yWindow="1300" windowWidth="25110" windowHeight="14640" tabRatio="765" xr2:uid="{CD11C47C-4470-47D7-8492-EF1E35E170CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed-IWG" sheetId="2" r:id="rId1"/>
@@ -1263,9 +1263,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CC3924-C92B-4F23-BF60-8291572759ED}">
   <dimension ref="A1:L333"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D288" sqref="D288"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E319" sqref="E319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1610,9 +1610,6 @@
       <c r="D21" s="3">
         <v>87.5</v>
       </c>
-      <c r="F21" s="3">
-        <v>1.36</v>
-      </c>
       <c r="G21" s="11">
         <v>857</v>
       </c>
@@ -6984,12 +6981,6 @@
       </c>
       <c r="C319" s="22">
         <v>40129</v>
-      </c>
-      <c r="E319" s="3">
-        <v>0</v>
-      </c>
-      <c r="F319" s="3">
-        <v>0</v>
       </c>
       <c r="K319" s="3">
         <f t="shared" si="9"/>
@@ -7258,7 +7249,7 @@
   <dimension ref="A1:H343"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
parameter changes for root organ update
</commit_message>
<xml_diff>
--- a/Prototypes/IntermediateWheatgrass/Observed.xlsx
+++ b/Prototypes/IntermediateWheatgrass/Observed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\USQ\PetesPapers\Thesis\Chapter5 PG Model\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\source\repos\ApsimX\Prototypes\IntermediateWheatgrass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6541F6D2-A841-4E36-8CCC-1E3552145CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA16A2C-49A8-4FB6-81C4-577075602E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="530" yWindow="1300" windowWidth="25110" windowHeight="14640" tabRatio="765" xr2:uid="{CD11C47C-4470-47D7-8492-EF1E35E170CD}"/>
+    <workbookView xWindow="350" yWindow="1830" windowWidth="21000" windowHeight="13740" tabRatio="765" xr2:uid="{CD11C47C-4470-47D7-8492-EF1E35E170CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed-IWG" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="81">
   <si>
     <t>SimulationName</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Total biomass calculated from grain/HI</t>
   </si>
 </sst>
 </file>
@@ -1263,9 +1266,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CC3924-C92B-4F23-BF60-8291572759ED}">
   <dimension ref="A1:L333"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E319" sqref="E319"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L307" sqref="L307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3608,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A129" s="9" t="s">
         <v>59</v>
       </c>
@@ -3626,7 +3629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A130" s="9" t="s">
         <v>59</v>
       </c>
@@ -3644,7 +3647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A131" s="9" t="s">
         <v>59</v>
       </c>
@@ -3662,7 +3665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A132" s="9" t="s">
         <v>59</v>
       </c>
@@ -3680,7 +3683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A133" s="9" t="s">
         <v>59</v>
       </c>
@@ -3698,7 +3701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A134" s="9" t="s">
         <v>59</v>
       </c>
@@ -3716,7 +3719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A135" s="9" t="s">
         <v>59</v>
       </c>
@@ -3745,8 +3748,11 @@
         <f t="shared" si="1"/>
         <v>17085.599999999999</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L135" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A136" s="9" t="s">
         <v>59</v>
       </c>
@@ -3765,7 +3771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A137" s="9" t="s">
         <v>59</v>
       </c>
@@ -3784,7 +3790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A138" s="9" t="s">
         <v>59</v>
       </c>
@@ -3803,7 +3809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A139" s="9" t="s">
         <v>59</v>
       </c>
@@ -3822,7 +3828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A140" s="9" t="s">
         <v>59</v>
       </c>
@@ -3841,7 +3847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A141" s="9" t="s">
         <v>59</v>
       </c>
@@ -3860,7 +3866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A142" s="9" t="s">
         <v>59</v>
       </c>
@@ -3879,7 +3885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A143" s="9" t="s">
         <v>59</v>
       </c>
@@ -3898,7 +3904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A144" s="9" t="s">
         <v>59</v>
       </c>
@@ -3917,7 +3923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A145" s="9" t="s">
         <v>59</v>
       </c>
@@ -3937,15 +3943,18 @@
         <f t="shared" si="1"/>
         <v>12763.2</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L145" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
       <c r="J146" s="3"/>
       <c r="K146" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A147" s="9" t="s">
         <v>5</v>
       </c>
@@ -3965,7 +3974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A148" s="11" t="s">
         <v>5</v>
       </c>
@@ -3984,7 +3993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A149" s="11" t="s">
         <v>5</v>
       </c>
@@ -4005,7 +4014,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A150" s="11" t="s">
         <v>5</v>
       </c>
@@ -4024,7 +4033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A151" s="11" t="s">
         <v>5</v>
       </c>
@@ -4043,7 +4052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A152" s="11" t="s">
         <v>5</v>
       </c>
@@ -4062,7 +4071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A153" s="11" t="s">
         <v>5</v>
       </c>
@@ -4081,7 +4090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A154" s="11" t="s">
         <v>5</v>
       </c>
@@ -4100,7 +4109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A155" s="11" t="s">
         <v>5</v>
       </c>
@@ -4119,7 +4128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A156" s="11" t="s">
         <v>5</v>
       </c>
@@ -4138,7 +4147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A157" s="11" t="s">
         <v>5</v>
       </c>
@@ -4157,7 +4166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A158" s="11" t="s">
         <v>5</v>
       </c>
@@ -4176,7 +4185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A159" s="11" t="s">
         <v>5</v>
       </c>
@@ -4195,7 +4204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A160" s="11" t="s">
         <v>5</v>
       </c>
@@ -6683,8 +6692,8 @@
         <v>42220</v>
       </c>
       <c r="E305" s="3">
-        <f>K305</f>
-        <v>14566.666666666668</v>
+        <f>J305</f>
+        <v>12666.666666666668</v>
       </c>
       <c r="F305" s="25">
         <v>760</v>
@@ -6711,8 +6720,8 @@
         <v>42586</v>
       </c>
       <c r="E306" s="3">
-        <f t="shared" ref="E306:E317" si="8">K306</f>
-        <v>6133.3333333333339</v>
+        <f t="shared" ref="E306:E317" si="8">J306</f>
+        <v>5333.3333333333339</v>
       </c>
       <c r="F306" s="25">
         <v>320</v>
@@ -6724,6 +6733,9 @@
         <f t="shared" ref="K306:K323" si="9">(J306*0.15)+J306</f>
         <v>6133.3333333333339</v>
       </c>
+      <c r="L306" s="11" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="307" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A307" s="21" t="s">
@@ -6737,7 +6749,7 @@
       </c>
       <c r="E307" s="3">
         <f t="shared" si="8"/>
-        <v>7484.1269841269841</v>
+        <v>6507.936507936508</v>
       </c>
       <c r="F307" s="25">
         <v>410</v>
@@ -6754,6 +6766,10 @@
       <c r="A308" s="21"/>
       <c r="B308" s="21"/>
       <c r="C308" s="22"/>
+      <c r="E308" s="3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="F308" s="25"/>
       <c r="J308" s="24"/>
       <c r="K308" s="3">
@@ -6772,6 +6788,7 @@
         <v>41887</v>
       </c>
       <c r="E309" s="3">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F309" s="25">
@@ -6795,7 +6812,7 @@
       </c>
       <c r="E310" s="3">
         <f t="shared" si="8"/>
-        <v>13540.322580645161</v>
+        <v>11774.193548387097</v>
       </c>
       <c r="F310" s="25">
         <v>730</v>
@@ -6820,7 +6837,7 @@
       </c>
       <c r="E311" s="3">
         <f t="shared" si="8"/>
-        <v>5290</v>
+        <v>4600</v>
       </c>
       <c r="F311" s="25">
         <v>230</v>
@@ -6845,7 +6862,7 @@
       </c>
       <c r="E312" s="3">
         <f t="shared" si="8"/>
-        <v>11500</v>
+        <v>10000</v>
       </c>
       <c r="F312" s="25">
         <v>660</v>
@@ -6862,6 +6879,10 @@
       <c r="A313" s="21"/>
       <c r="B313" s="21"/>
       <c r="C313" s="22"/>
+      <c r="E313" s="3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="F313" s="25"/>
       <c r="J313" s="24"/>
       <c r="K313" s="3">
@@ -6880,6 +6901,7 @@
         <v>41887</v>
       </c>
       <c r="E314" s="3">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F314" s="25">
@@ -6903,7 +6925,7 @@
       </c>
       <c r="E315" s="3">
         <f t="shared" si="8"/>
-        <v>11960</v>
+        <v>10400</v>
       </c>
       <c r="F315" s="25">
         <v>780</v>
@@ -6928,7 +6950,7 @@
       </c>
       <c r="E316" s="3">
         <f t="shared" si="8"/>
-        <v>6078.5714285714284</v>
+        <v>5285.7142857142853</v>
       </c>
       <c r="F316" s="25">
         <v>370</v>
@@ -6953,7 +6975,7 @@
       </c>
       <c r="E317" s="3">
         <f t="shared" si="8"/>
-        <v>8138.461538461539</v>
+        <v>7076.9230769230771</v>
       </c>
       <c r="F317" s="25">
         <v>460</v>

</xml_diff>